<commit_message>
added csv to data folder
</commit_message>
<xml_diff>
--- a/data/PhD_DS_Exp1.xlsx
+++ b/data/PhD_DS_Exp1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bc0e8b02e11dad1/Documents/GitHub/minerva2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{6198A103-80E3-451C-A067-65BA52B2B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91917190-6EAE-4D46-9D16-0AB19E8FF700}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{6198A103-80E3-451C-A067-65BA52B2B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5891DE7-CB1A-4F61-8364-A5FD1D12AC57}"/>
   <bookViews>
-    <workbookView xWindow="83100" yWindow="5475" windowWidth="13005" windowHeight="20985" activeTab="1" xr2:uid="{427DD094-3641-4A0A-B292-8D5F2670F49C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{427DD094-3641-4A0A-B292-8D5F2670F49C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$322</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$O$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$L$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="701">
   <si>
     <t>chase dream</t>
   </si>
@@ -1808,15 +1808,6 @@
   </si>
   <si>
     <t>race</t>
-  </si>
-  <si>
-    <t>syn</t>
-  </si>
-  <si>
-    <t>syn_freq</t>
-  </si>
-  <si>
-    <t>syn_score</t>
   </si>
   <si>
     <t>desert</t>
@@ -2188,9 +2179,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2206,6 +2196,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4414,15 +4408,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464C3685-9491-42ED-85B1-DFA0B214114C}">
-  <dimension ref="A1:O118"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.20703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.15625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.15625" customWidth="1"/>
     <col min="4" max="4" width="8.7890625" bestFit="1" customWidth="1"/>
@@ -4432,11 +4426,10 @@
     <col min="9" max="9" width="10.47265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7890625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7890625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="11.7890625" customWidth="1"/>
-    <col min="15" max="15" width="68.7890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="68.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -4444,7 +4437,7 @@
         <v>342</v>
       </c>
       <c r="C1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D1" t="s">
         <v>340</v>
@@ -4471,24 +4464,18 @@
         <v>347</v>
       </c>
       <c r="L1" t="s">
-        <v>589</v>
-      </c>
-      <c r="M1" t="s">
-        <v>590</v>
-      </c>
-      <c r="N1" t="s">
-        <v>591</v>
-      </c>
-      <c r="O1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D2">
         <v>19302</v>
@@ -4514,48 +4501,51 @@
       <c r="K2">
         <v>7.9</v>
       </c>
-      <c r="L2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" t="s">
+        <v>617</v>
+      </c>
+      <c r="D3">
         <v>4809</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>6.5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>356</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
         <v>3316</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>6.4</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>357</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3">
         <v>4244</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>306</v>
       </c>
       <c r="C4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D4">
         <v>12754</v>
@@ -4582,12 +4572,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D5">
         <v>14612</v>
@@ -4614,12 +4607,15 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>577</v>
       </c>
       <c r="C6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D6">
         <v>58033</v>
@@ -4646,12 +4642,15 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>362</v>
       </c>
       <c r="C7" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D7">
         <v>53167</v>
@@ -4678,12 +4677,15 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>416</v>
       </c>
       <c r="C8" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D8">
         <v>79084</v>
@@ -4710,12 +4712,15 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>366</v>
       </c>
       <c r="C9" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D9">
         <v>10061</v>
@@ -4742,12 +4747,15 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>421</v>
       </c>
       <c r="C10" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D10">
         <v>44571</v>
@@ -4774,12 +4782,15 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>499</v>
       </c>
       <c r="C11" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D11">
         <v>56812</v>
@@ -4806,12 +4817,15 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>369</v>
       </c>
       <c r="C12" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D12">
         <v>133801</v>
@@ -4837,27 +4851,33 @@
       <c r="K12">
         <v>9.6999999999999993</v>
       </c>
-      <c r="O12" t="s">
+      <c r="L12" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>279</v>
       </c>
       <c r="C13" t="s">
-        <v>675</v>
-      </c>
-      <c r="O13" t="s">
+        <v>672</v>
+      </c>
+      <c r="L13" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D14">
         <v>15269</v>
@@ -4883,27 +4903,33 @@
       <c r="K14">
         <v>8.5</v>
       </c>
-      <c r="O14" t="s">
+      <c r="L14" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>327</v>
       </c>
       <c r="C15" t="s">
-        <v>676</v>
-      </c>
-      <c r="O15" t="s">
+        <v>673</v>
+      </c>
+      <c r="L15" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>352</v>
       </c>
       <c r="C16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D16">
         <v>58741</v>
@@ -4930,12 +4956,15 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>377</v>
       </c>
       <c r="C17" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D17">
         <v>7983</v>
@@ -4961,16 +4990,19 @@
       <c r="K17">
         <v>5</v>
       </c>
-      <c r="O17" t="s">
+      <c r="L17" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>332</v>
       </c>
       <c r="C18" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D18">
         <v>1110</v>
@@ -4997,12 +5029,15 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>331</v>
       </c>
       <c r="C19" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D19">
         <v>46036</v>
@@ -5029,12 +5064,15 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>387</v>
       </c>
       <c r="C20" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D20">
         <v>3854</v>
@@ -5060,16 +5098,19 @@
       <c r="K20">
         <v>6.9</v>
       </c>
-      <c r="O20" t="s">
+      <c r="L20" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D21">
         <v>40766</v>
@@ -5095,16 +5136,19 @@
       <c r="K21">
         <v>8.4</v>
       </c>
-      <c r="O21" t="s">
+      <c r="L21" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D22">
         <v>15306</v>
@@ -5122,12 +5166,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>574</v>
       </c>
       <c r="C23" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D23">
         <v>447</v>
@@ -5154,12 +5201,15 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D24">
         <v>13808</v>
@@ -5168,12 +5218,15 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25" t="s">
         <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D25">
         <v>10447</v>
@@ -5199,16 +5252,19 @@
       <c r="K25">
         <v>3.7</v>
       </c>
-      <c r="O25" t="s">
+      <c r="L25" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
         <v>406</v>
       </c>
       <c r="C26" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D26">
         <v>1228</v>
@@ -5235,20 +5291,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="B27" t="s">
         <v>277</v>
       </c>
       <c r="C27" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>27</v>
+      </c>
       <c r="B28" t="s">
         <v>400</v>
       </c>
       <c r="C28" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D28">
         <v>4620</v>
@@ -5274,16 +5336,19 @@
       <c r="K28">
         <v>6.6</v>
       </c>
-      <c r="O28" t="s">
+      <c r="L28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>28</v>
+      </c>
       <c r="B29" t="s">
         <v>233</v>
       </c>
       <c r="C29" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D29">
         <v>6378</v>
@@ -5301,12 +5366,15 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>29</v>
+      </c>
       <c r="B30" t="s">
         <v>486</v>
       </c>
       <c r="C30" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D30">
         <v>5871</v>
@@ -5332,16 +5400,19 @@
       <c r="K30">
         <v>4.0999999999999996</v>
       </c>
-      <c r="O30" t="s">
+      <c r="L30" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="B31" t="s">
         <v>404</v>
       </c>
       <c r="C31" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D31">
         <v>2706</v>
@@ -5368,12 +5439,15 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>31</v>
+      </c>
       <c r="B32" t="s">
         <v>411</v>
       </c>
       <c r="C32" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D32">
         <v>58610</v>
@@ -5391,12 +5465,15 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>32</v>
+      </c>
       <c r="B33" t="s">
         <v>415</v>
       </c>
       <c r="C33" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D33">
         <v>15554</v>
@@ -5423,12 +5500,15 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>33</v>
+      </c>
       <c r="B34" t="s">
         <v>419</v>
       </c>
       <c r="C34" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="D34">
         <v>44358</v>
@@ -5446,20 +5526,26 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>34</v>
+      </c>
       <c r="B35" t="s">
         <v>144</v>
       </c>
       <c r="C35" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>35</v>
+      </c>
       <c r="B36" t="s">
         <v>247</v>
       </c>
       <c r="C36" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D36">
         <v>35716</v>
@@ -5486,12 +5572,15 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>36</v>
+      </c>
       <c r="B37" t="s">
         <v>427</v>
       </c>
       <c r="C37" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D37">
         <v>5499</v>
@@ -5518,12 +5607,15 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>37</v>
+      </c>
       <c r="B38" t="s">
         <v>430</v>
       </c>
       <c r="C38" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D38">
         <v>24588</v>
@@ -5549,16 +5641,19 @@
       <c r="K38">
         <v>7.3</v>
       </c>
-      <c r="O38" t="s">
+      <c r="L38" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>38</v>
+      </c>
       <c r="B39" t="s">
         <v>405</v>
       </c>
       <c r="C39" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D39">
         <v>652</v>
@@ -5576,12 +5671,15 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>39</v>
+      </c>
       <c r="B40" t="s">
         <v>431</v>
       </c>
       <c r="C40" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D40">
         <v>23036</v>
@@ -5608,12 +5706,15 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>40</v>
+      </c>
       <c r="B41" t="s">
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D41">
         <v>14114</v>
@@ -5639,16 +5740,19 @@
       <c r="K41">
         <v>8.4</v>
       </c>
-      <c r="O41" t="s">
+      <c r="L41" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>41</v>
+      </c>
       <c r="B42" t="s">
         <v>436</v>
       </c>
       <c r="C42" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D42">
         <v>1404</v>
@@ -5675,12 +5779,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>42</v>
+      </c>
       <c r="B43" t="s">
         <v>180</v>
       </c>
       <c r="C43" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D43">
         <v>6865</v>
@@ -5707,12 +5814,15 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>43</v>
+      </c>
       <c r="B44" t="s">
         <v>128</v>
       </c>
       <c r="C44" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D44">
         <v>9599</v>
@@ -5738,16 +5848,19 @@
       <c r="K44">
         <v>3.9</v>
       </c>
-      <c r="O44" t="s">
+      <c r="L44" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>44</v>
+      </c>
       <c r="B45" t="s">
         <v>481</v>
       </c>
       <c r="C45" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D45">
         <v>6358</v>
@@ -5774,12 +5887,15 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>45</v>
+      </c>
       <c r="B46" t="s">
         <v>440</v>
       </c>
       <c r="C46" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D46">
         <v>2450</v>
@@ -5797,12 +5913,15 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="B47" t="s">
         <v>311</v>
       </c>
       <c r="C47" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D47">
         <v>1451</v>
@@ -5820,12 +5939,15 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>47</v>
+      </c>
       <c r="B48" t="s">
         <v>444</v>
       </c>
       <c r="C48" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D48">
         <v>113164</v>
@@ -5851,16 +5973,19 @@
       <c r="K48">
         <v>7.2</v>
       </c>
-      <c r="O48" t="s">
+      <c r="L48" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>48</v>
+      </c>
       <c r="B49" t="s">
         <v>109</v>
       </c>
       <c r="C49" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D49">
         <v>3968</v>
@@ -5878,12 +6003,15 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>49</v>
+      </c>
       <c r="B50" t="s">
         <v>565</v>
       </c>
       <c r="C50" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D50">
         <v>11397</v>
@@ -5909,16 +6037,19 @@
       <c r="K50">
         <v>5.9</v>
       </c>
-      <c r="O50" t="s">
+      <c r="L50" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
       <c r="B51" t="s">
         <v>448</v>
       </c>
       <c r="C51" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D51">
         <v>2905</v>
@@ -5945,12 +6076,15 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
       <c r="B52" t="s">
         <v>451</v>
       </c>
       <c r="C52" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D52">
         <v>2090</v>
@@ -5976,16 +6110,19 @@
       <c r="K52">
         <v>7.8</v>
       </c>
-      <c r="O52" t="s">
+      <c r="L52" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
       <c r="B53" t="s">
         <v>263</v>
       </c>
       <c r="C53" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D53">
         <v>10490</v>
@@ -6012,12 +6149,15 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
       <c r="B54" t="s">
         <v>381</v>
       </c>
       <c r="C54" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D54">
         <v>30145</v>
@@ -6035,12 +6175,15 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
       <c r="B55" t="s">
         <v>147</v>
       </c>
       <c r="C55" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D55">
         <v>5574</v>
@@ -6058,12 +6201,15 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
       <c r="B56" t="s">
         <v>458</v>
       </c>
       <c r="C56" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D56">
         <v>23341</v>
@@ -6081,12 +6227,15 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
       <c r="B57" t="s">
         <v>460</v>
       </c>
       <c r="C57" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D57">
         <v>13271</v>
@@ -6104,12 +6253,15 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
       <c r="B58" t="s">
         <v>461</v>
       </c>
       <c r="C58" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D58">
         <v>7240</v>
@@ -6127,12 +6279,15 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
       <c r="B59" t="s">
         <v>491</v>
       </c>
       <c r="C59" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D59">
         <v>9233</v>
@@ -6159,12 +6314,15 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
       <c r="B60" t="s">
         <v>291</v>
       </c>
       <c r="C60" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D60">
         <v>32844</v>
@@ -6191,12 +6349,15 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
       <c r="B61" t="s">
         <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D61">
         <v>26037</v>
@@ -6223,12 +6384,15 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
       <c r="B62" t="s">
         <v>464</v>
       </c>
       <c r="C62" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D62">
         <v>709</v>
@@ -6255,12 +6419,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
       <c r="B63" t="s">
         <v>467</v>
       </c>
       <c r="C63" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D63">
         <v>12323</v>
@@ -6287,12 +6454,15 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
       <c r="B64" t="s">
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D64">
         <v>1318</v>
@@ -6310,12 +6480,15 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
       <c r="B65" t="s">
         <v>569</v>
       </c>
       <c r="C65" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D65">
         <v>1157</v>
@@ -6342,12 +6515,15 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>65</v>
+      </c>
       <c r="B66" t="s">
         <v>470</v>
       </c>
       <c r="C66" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D66">
         <v>96351</v>
@@ -6374,12 +6550,15 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>66</v>
+      </c>
       <c r="B67" t="s">
         <v>326</v>
       </c>
       <c r="C67" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D67">
         <v>25712</v>
@@ -6406,12 +6585,15 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>67</v>
+      </c>
       <c r="B68" t="s">
         <v>328</v>
       </c>
       <c r="C68" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D68">
         <v>1797</v>
@@ -6438,12 +6620,15 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>68</v>
+      </c>
       <c r="B69" t="s">
         <v>476</v>
       </c>
       <c r="C69" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D69">
         <v>24213</v>
@@ -6461,12 +6646,15 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>69</v>
+      </c>
       <c r="B70" t="s">
         <v>477</v>
       </c>
       <c r="C70" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D70">
         <v>6897</v>
@@ -6484,12 +6672,15 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>70</v>
+      </c>
       <c r="B71" t="s">
         <v>479</v>
       </c>
       <c r="C71" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D71">
         <v>4607</v>
@@ -6516,12 +6707,15 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>71</v>
+      </c>
       <c r="B72" t="s">
         <v>167</v>
       </c>
       <c r="C72" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D72">
         <v>28530</v>
@@ -6548,12 +6742,15 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>72</v>
+      </c>
       <c r="B73" t="s">
         <v>325</v>
       </c>
       <c r="C73" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D73">
         <v>1072</v>
@@ -6571,12 +6768,15 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>73</v>
+      </c>
       <c r="B74" t="s">
         <v>489</v>
       </c>
       <c r="C74" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D74">
         <v>168326</v>
@@ -6603,12 +6803,15 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>74</v>
+      </c>
       <c r="B75" t="s">
         <v>268</v>
       </c>
       <c r="C75" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D75">
         <v>34479</v>
@@ -6626,12 +6829,15 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>75</v>
+      </c>
       <c r="B76" t="s">
         <v>322</v>
       </c>
       <c r="C76" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D76">
         <v>22091</v>
@@ -6649,12 +6855,15 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>76</v>
+      </c>
       <c r="B77" t="s">
         <v>329</v>
       </c>
       <c r="C77" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D77">
         <v>8708</v>
@@ -6672,12 +6881,15 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>77</v>
+      </c>
       <c r="B78" t="s">
         <v>333</v>
       </c>
       <c r="C78" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D78">
         <v>1286</v>
@@ -6704,12 +6916,15 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
+        <v>78</v>
+      </c>
       <c r="B79" t="s">
         <v>495</v>
       </c>
       <c r="C79" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D79">
         <v>4057</v>
@@ -6727,12 +6942,15 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
+        <v>79</v>
+      </c>
       <c r="B80" t="s">
         <v>353</v>
       </c>
       <c r="C80" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D80">
         <v>17250</v>
@@ -6759,12 +6977,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>80</v>
+      </c>
       <c r="B81" t="s">
         <v>337</v>
       </c>
       <c r="C81" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D81">
         <v>2665</v>
@@ -6791,12 +7012,15 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>81</v>
+      </c>
       <c r="B82" t="s">
         <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D82">
         <v>11839</v>
@@ -6823,12 +7047,15 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>82</v>
+      </c>
       <c r="B83" t="s">
         <v>500</v>
       </c>
       <c r="C83" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D83">
         <v>3129</v>
@@ -6854,16 +7081,19 @@
       <c r="K83">
         <v>9.6</v>
       </c>
-      <c r="O83" t="s">
+      <c r="L83" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>83</v>
+      </c>
       <c r="B84" t="s">
         <v>504</v>
       </c>
       <c r="C84" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D84">
         <v>8437</v>
@@ -6889,16 +7119,19 @@
       <c r="K84">
         <v>6.3</v>
       </c>
-      <c r="O84" t="s">
+      <c r="L84" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>84</v>
+      </c>
       <c r="B85" t="s">
         <v>301</v>
       </c>
       <c r="C85" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D85">
         <v>2277</v>
@@ -6924,16 +7157,19 @@
       <c r="K85">
         <v>6.3</v>
       </c>
-      <c r="O85" t="s">
+      <c r="L85" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
+        <v>85</v>
+      </c>
       <c r="B86" t="s">
         <v>508</v>
       </c>
       <c r="C86" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D86">
         <v>4420</v>
@@ -6959,16 +7195,19 @@
       <c r="K86">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O86" t="s">
+      <c r="L86" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>86</v>
+      </c>
       <c r="B87" t="s">
         <v>114</v>
       </c>
       <c r="C87" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="D87">
         <v>1085</v>
@@ -6994,16 +7233,19 @@
       <c r="K87">
         <v>5.6</v>
       </c>
-      <c r="O87" t="s">
+      <c r="L87" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
+        <v>87</v>
+      </c>
       <c r="B88" t="s">
         <v>320</v>
       </c>
       <c r="C88" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D88">
         <v>2087</v>
@@ -7030,7 +7272,10 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>88</v>
+      </c>
       <c r="B89" t="s">
         <v>39</v>
       </c>
@@ -7062,12 +7307,15 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>89</v>
+      </c>
       <c r="B90" t="s">
         <v>272</v>
       </c>
       <c r="C90" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D90">
         <v>3504</v>
@@ -7093,16 +7341,19 @@
       <c r="K90">
         <v>10.9</v>
       </c>
-      <c r="O90" t="s">
+      <c r="L90" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>90</v>
+      </c>
       <c r="B91" t="s">
         <v>522</v>
       </c>
       <c r="C91" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D91">
         <v>1203</v>
@@ -7128,16 +7379,19 @@
       <c r="K91">
         <v>6.5</v>
       </c>
-      <c r="O91" t="s">
+      <c r="L91" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>91</v>
+      </c>
       <c r="B92" t="s">
         <v>529</v>
       </c>
       <c r="C92" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D92">
         <v>2021</v>
@@ -7164,12 +7418,15 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>92</v>
+      </c>
       <c r="B93" t="s">
         <v>156</v>
       </c>
       <c r="C93" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D93">
         <v>2935</v>
@@ -7196,12 +7453,15 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>93</v>
+      </c>
       <c r="B94" t="s">
         <v>330</v>
       </c>
       <c r="C94" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D94">
         <v>8646</v>
@@ -7228,12 +7488,15 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>94</v>
+      </c>
       <c r="B95" t="s">
         <v>236</v>
       </c>
       <c r="C95" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D95">
         <v>4067</v>
@@ -7251,12 +7514,15 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>95</v>
+      </c>
       <c r="B96" t="s">
         <v>530</v>
       </c>
       <c r="C96" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D96">
         <v>3270</v>
@@ -7283,12 +7549,15 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>96</v>
+      </c>
       <c r="B97" t="s">
         <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D97">
         <v>4677</v>
@@ -7306,12 +7575,15 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>97</v>
+      </c>
       <c r="B98" t="s">
         <v>534</v>
       </c>
       <c r="C98" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D98">
         <v>2974</v>
@@ -7338,12 +7610,15 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>98</v>
+      </c>
       <c r="B99" t="s">
         <v>334</v>
       </c>
       <c r="C99" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D99">
         <v>28332</v>
@@ -7370,12 +7645,15 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>99</v>
+      </c>
       <c r="B100" t="s">
         <v>537</v>
       </c>
       <c r="C100" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D100">
         <v>6065</v>
@@ -7402,12 +7680,15 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>100</v>
+      </c>
       <c r="B101" t="s">
         <v>539</v>
       </c>
       <c r="C101" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D101">
         <v>5144</v>
@@ -7434,12 +7715,15 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102">
+        <v>101</v>
+      </c>
       <c r="B102" t="s">
         <v>543</v>
       </c>
       <c r="C102" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D102">
         <v>13132</v>
@@ -7466,12 +7750,15 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103">
+        <v>102</v>
+      </c>
       <c r="B103" t="s">
         <v>298</v>
       </c>
       <c r="C103" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D103">
         <v>8341</v>
@@ -7489,12 +7776,15 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104">
+        <v>103</v>
+      </c>
       <c r="B104" t="s">
         <v>105</v>
       </c>
       <c r="C104" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D104">
         <v>2692</v>
@@ -7512,7 +7802,10 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
+        <v>104</v>
+      </c>
       <c r="B105" t="s">
         <v>171</v>
       </c>
@@ -7535,12 +7828,15 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="106" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106">
+        <v>105</v>
+      </c>
       <c r="B106" t="s">
         <v>548</v>
       </c>
       <c r="C106" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D106">
         <v>14277</v>
@@ -7558,12 +7854,15 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="107" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107">
+        <v>106</v>
+      </c>
       <c r="B107" t="s">
         <v>87</v>
       </c>
       <c r="C107" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D107">
         <v>4956</v>
@@ -7590,12 +7889,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108">
+        <v>107</v>
+      </c>
       <c r="B108" t="s">
         <v>324</v>
       </c>
       <c r="C108" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D108">
         <v>58685</v>
@@ -7622,12 +7924,15 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="109" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109">
+        <v>108</v>
+      </c>
       <c r="B109" t="s">
         <v>552</v>
       </c>
       <c r="C109" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D109">
         <v>6271</v>
@@ -7654,12 +7959,15 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="110" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110">
+        <v>109</v>
+      </c>
       <c r="B110" t="s">
         <v>556</v>
       </c>
       <c r="C110" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D110">
         <v>1111</v>
@@ -7686,12 +7994,15 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="111" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111">
+        <v>110</v>
+      </c>
       <c r="B111" t="s">
         <v>242</v>
       </c>
       <c r="C111" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D111">
         <v>3432</v>
@@ -7717,16 +8028,19 @@
       <c r="K111">
         <v>6.8</v>
       </c>
-      <c r="O111" t="s">
+      <c r="L111" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="112" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112">
+        <v>111</v>
+      </c>
       <c r="B112" t="s">
         <v>560</v>
       </c>
       <c r="C112" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="D112">
         <v>27122</v>
@@ -7753,12 +8067,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
+        <v>112</v>
+      </c>
       <c r="B113" t="s">
         <v>561</v>
       </c>
       <c r="C113" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D113">
         <v>15961</v>
@@ -7785,12 +8102,15 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
+        <v>113</v>
+      </c>
       <c r="B114" t="s">
         <v>579</v>
       </c>
       <c r="C114" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D114">
         <v>4510</v>
@@ -7817,7 +8137,10 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <v>114</v>
+      </c>
       <c r="B115" t="s">
         <v>580</v>
       </c>
@@ -7848,16 +8171,19 @@
       <c r="K115">
         <v>10.9</v>
       </c>
-      <c r="O115" t="s">
+      <c r="L115" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
+        <v>115</v>
+      </c>
       <c r="B116" t="s">
         <v>582</v>
       </c>
       <c r="C116" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="D116">
         <v>8402</v>
@@ -7884,12 +8210,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
+        <v>116</v>
+      </c>
       <c r="B117" t="s">
         <v>584</v>
       </c>
       <c r="C117" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D117">
         <v>27515</v>
@@ -7916,12 +8245,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118">
+        <v>117</v>
+      </c>
       <c r="B118" t="s">
         <v>586</v>
       </c>
       <c r="C118" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D118">
         <v>42155</v>
@@ -7949,8 +8281,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O118" xr:uid="{464C3685-9491-42ED-85B1-DFA0B214114C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O113">
+  <autoFilter ref="A1:L118" xr:uid="{464C3685-9491-42ED-85B1-DFA0B214114C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L113">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added new stimulifile with idioms
</commit_message>
<xml_diff>
--- a/data/PhD_DS_Exp1.xlsx
+++ b/data/PhD_DS_Exp1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bc0e8b02e11dad1/Documents/GitHub/minerva2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{6198A103-80E3-451C-A067-65BA52B2B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5891DE7-CB1A-4F61-8364-A5FD1D12AC57}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{6198A103-80E3-451C-A067-65BA52B2B5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9195B8A7-AD3F-4093-B620-A4D962F5C1E6}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{427DD094-3641-4A0A-B292-8D5F2670F49C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{427DD094-3641-4A0A-B292-8D5F2670F49C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2159,12 +2159,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2179,8 +2185,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2196,10 +2203,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2506,12 +2509,12 @@
       <selection activeCell="B1" sqref="B1:B315"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>188</v>
       </c>
@@ -2519,27 +2522,27 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -2555,17 +2558,17 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>306</v>
       </c>
@@ -2573,12 +2576,12 @@
         <v>306</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -2586,17 +2589,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>255</v>
       </c>
@@ -2604,17 +2607,17 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2622,22 +2625,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -2645,17 +2648,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>279</v>
       </c>
@@ -2663,42 +2666,42 @@
         <v>279</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2706,47 +2709,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2754,7 +2757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -2762,17 +2765,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>197</v>
       </c>
@@ -2788,27 +2791,27 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -2816,17 +2819,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>23</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -2842,12 +2845,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>277</v>
       </c>
@@ -2855,27 +2858,27 @@
         <v>277</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>51</v>
       </c>
@@ -2883,17 +2886,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>233</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -2909,17 +2912,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>165</v>
       </c>
@@ -2927,12 +2930,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -2940,17 +2943,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>132</v>
       </c>
@@ -2958,17 +2961,17 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -2976,12 +2979,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>144</v>
       </c>
@@ -2989,17 +2992,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>183</v>
       </c>
@@ -3007,12 +3010,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -3028,32 +3031,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -3061,17 +3064,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>257</v>
       </c>
@@ -3079,12 +3082,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>79</v>
       </c>
@@ -3092,17 +3095,17 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>314</v>
       </c>
@@ -3110,27 +3113,27 @@
         <v>314</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>180</v>
       </c>
@@ -3138,22 +3141,22 @@
         <v>180</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -3161,27 +3164,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>29</v>
       </c>
@@ -3189,12 +3192,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>292</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -3210,42 +3213,42 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>195</v>
       </c>
@@ -3253,17 +3256,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>239</v>
       </c>
@@ -3271,17 +3274,17 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>201</v>
       </c>
@@ -3289,12 +3292,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>158</v>
       </c>
@@ -3302,42 +3305,42 @@
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>263</v>
       </c>
@@ -3345,17 +3348,17 @@
         <v>263</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>214</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>20</v>
       </c>
@@ -3371,17 +3374,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>153</v>
       </c>
@@ -3389,32 +3392,32 @@
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>291</v>
       </c>
@@ -3422,17 +3425,17 @@
         <v>291</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>309</v>
       </c>
@@ -3440,12 +3443,12 @@
         <v>309</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>312</v>
       </c>
@@ -3453,37 +3456,37 @@
         <v>312</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>297</v>
       </c>
@@ -3491,22 +3494,22 @@
         <v>297</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>81</v>
       </c>
@@ -3514,27 +3517,27 @@
         <v>81</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>62</v>
       </c>
@@ -3542,27 +3545,27 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>69</v>
       </c>
@@ -3570,12 +3573,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>281</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>273</v>
       </c>
@@ -3591,22 +3594,22 @@
         <v>273</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>167</v>
       </c>
@@ -3614,17 +3617,17 @@
         <v>167</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>13</v>
       </c>
@@ -3632,22 +3635,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>268</v>
       </c>
@@ -3655,27 +3658,27 @@
         <v>268</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>310</v>
       </c>
@@ -3683,67 +3686,67 @@
         <v>310</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>96</v>
       </c>
@@ -3751,7 +3754,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>300</v>
       </c>
@@ -3759,17 +3762,17 @@
         <v>322</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>9</v>
       </c>
@@ -3777,12 +3780,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>222</v>
       </c>
@@ -3790,17 +3793,17 @@
         <v>222</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>321</v>
       </c>
@@ -3808,17 +3811,17 @@
         <v>321</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>301</v>
       </c>
@@ -3826,17 +3829,17 @@
         <v>301</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>129</v>
       </c>
@@ -3844,27 +3847,27 @@
         <v>129</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>114</v>
       </c>
@@ -3872,12 +3875,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>320</v>
       </c>
@@ -3885,47 +3888,47 @@
         <v>320</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>39</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>136</v>
       </c>
@@ -3941,22 +3944,22 @@
         <v>136</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>200</v>
       </c>
@@ -3964,27 +3967,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>305</v>
       </c>
@@ -3992,22 +3995,22 @@
         <v>305</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>156</v>
       </c>
@@ -4015,17 +4018,17 @@
         <v>156</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>236</v>
       </c>
@@ -4033,12 +4036,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>113</v>
       </c>
@@ -4046,7 +4049,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>102</v>
       </c>
@@ -4054,12 +4057,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>137</v>
       </c>
@@ -4067,17 +4070,17 @@
         <v>137</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>276</v>
       </c>
@@ -4085,27 +4088,27 @@
         <v>323</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>84</v>
       </c>
@@ -4113,17 +4116,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>298</v>
       </c>
@@ -4131,7 +4134,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>238</v>
       </c>
@@ -4139,52 +4142,52 @@
         <v>238</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>108</v>
       </c>
@@ -4192,22 +4195,22 @@
         <v>108</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>119</v>
       </c>
@@ -4215,7 +4218,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>150</v>
       </c>
@@ -4223,37 +4226,37 @@
         <v>150</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>162</v>
       </c>
@@ -4261,7 +4264,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>77</v>
       </c>
@@ -4269,37 +4272,37 @@
         <v>324</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>202</v>
       </c>
@@ -4307,17 +4310,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>230</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>242</v>
       </c>
@@ -4333,22 +4336,22 @@
         <v>242</v>
       </c>
     </row>
-    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>175</v>
       </c>
@@ -4356,37 +4359,37 @@
         <v>175</v>
       </c>
     </row>
-    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="321" spans="1:1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="322" spans="1:1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>294</v>
       </c>
@@ -4408,28 +4411,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464C3685-9491-42ED-85B1-DFA0B214114C}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.20703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.15625" customWidth="1"/>
-    <col min="4" max="4" width="8.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5234375" customWidth="1"/>
-    <col min="9" max="9" width="10.47265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7890625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7890625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="68.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="68.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>335</v>
       </c>
@@ -4467,7 +4471,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4502,7 +4506,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4537,7 +4541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4572,7 +4576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4607,7 +4611,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4642,7 +4646,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4677,7 +4681,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4712,7 +4716,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4747,7 +4751,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4782,7 +4786,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4817,7 +4821,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4855,7 +4859,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4869,7 +4873,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4907,7 +4911,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4921,7 +4925,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4956,7 +4960,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4994,7 +4998,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5029,7 +5033,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5064,7 +5068,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5102,7 +5106,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5140,7 +5144,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5166,7 +5170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5201,7 +5205,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5218,7 +5222,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5256,7 +5260,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5291,7 +5295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5302,7 +5306,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5340,7 +5344,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5366,7 +5370,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5404,7 +5408,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5439,7 +5443,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5465,7 +5469,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5500,7 +5504,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5526,7 +5530,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5537,7 +5541,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5572,7 +5576,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5607,7 +5611,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5645,7 +5649,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5671,7 +5675,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5706,7 +5710,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5744,7 +5748,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5779,7 +5783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5814,7 +5818,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5852,7 +5856,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5887,7 +5891,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5913,7 +5917,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5939,7 +5943,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5977,7 +5981,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6003,7 +6007,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6041,7 +6045,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6076,7 +6080,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6114,7 +6118,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6149,7 +6153,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6175,7 +6179,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6201,7 +6205,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6227,7 +6231,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6253,7 +6257,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6279,7 +6283,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6314,7 +6318,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6349,7 +6353,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6384,7 +6388,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6419,7 +6423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6454,7 +6458,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6480,7 +6484,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6515,7 +6519,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6550,7 +6554,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6585,7 +6589,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6620,7 +6624,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6646,7 +6650,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6672,7 +6676,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6707,7 +6711,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6742,7 +6746,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6768,7 +6772,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6803,7 +6807,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6829,7 +6833,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6855,7 +6859,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6881,7 +6885,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6916,7 +6920,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6942,7 +6946,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6977,7 +6981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7012,7 +7016,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7047,83 +7051,83 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83">
+    <row r="83" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>3129</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="1">
         <v>7.1</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="1">
         <v>12799</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="1">
         <v>7.6</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="J83">
+      <c r="J83" s="1">
         <v>9062</v>
       </c>
-      <c r="K83">
+      <c r="K83" s="1">
         <v>9.6</v>
       </c>
-      <c r="L83" t="s">
+      <c r="L83" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84">
+    <row r="84" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>8437</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="1">
         <v>4595</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="1">
         <v>7.7</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="J84">
+      <c r="J84" s="1">
         <v>4297</v>
       </c>
-      <c r="K84">
+      <c r="K84" s="1">
         <v>6.3</v>
       </c>
-      <c r="L84" t="s">
+      <c r="L84" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7161,45 +7165,45 @@
         <v>514</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86">
+    <row r="86" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>4420</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="1">
         <v>8.1</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="1">
         <v>2869</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="1">
         <v>8.1</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="J86">
+      <c r="J86" s="1">
         <v>1279</v>
       </c>
-      <c r="K86">
+      <c r="K86" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L86" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7237,7 +7241,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7272,7 +7276,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7307,7 +7311,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -7345,7 +7349,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -7383,7 +7387,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7418,7 +7422,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -7453,7 +7457,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -7488,7 +7492,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -7514,7 +7518,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -7549,7 +7553,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -7575,7 +7579,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -7610,7 +7614,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -7645,7 +7649,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -7680,7 +7684,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -7715,7 +7719,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -7750,7 +7754,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -7776,7 +7780,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -7802,7 +7806,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -7828,7 +7832,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -7854,7 +7858,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7889,7 +7893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7924,7 +7928,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7959,7 +7963,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7994,7 +7998,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -8032,7 +8036,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -8067,7 +8071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -8102,7 +8106,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -8137,7 +8141,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -8175,7 +8179,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -8210,7 +8214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -8245,7 +8249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -8282,6 +8286,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L118" xr:uid="{464C3685-9491-42ED-85B1-DFA0B214114C}">
+    <filterColumn colId="8">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L113">
       <sortCondition ref="B1"/>
     </sortState>

</xml_diff>